<commit_message>
added support for ip ranges and port ranges
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2446E34E-F952-4ECF-A37D-BED4B3FF2474}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C83C4A-45C4-4285-B791-433FF075165D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="4" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="FirewallPolicies" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -287,6 +287,24 @@
   </si>
   <si>
     <t>'test_tcp','test_udp','test2_tcp'</t>
+  </si>
+  <si>
+    <t>test29</t>
+  </si>
+  <si>
+    <t>test30</t>
+  </si>
+  <si>
+    <t>1.1.1.1-10.10.10.10</t>
+  </si>
+  <si>
+    <t>20.20.20.20-30.30.30.30</t>
+  </si>
+  <si>
+    <t>test_range</t>
+  </si>
+  <si>
+    <t>1000-2000</t>
   </si>
 </sst>
 </file>
@@ -659,7 +677,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -723,13 +741,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2D0E66-9821-4420-9073-ECB8C986F385}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
@@ -961,6 +982,22 @@
       </c>
       <c r="B29" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1013,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F0D103-70F1-467C-A4A0-6C4FAD2E3DAB}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1070,6 +1107,17 @@
         <v>1456</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1079,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6472A306-4237-4364-B563-EDDE513583A6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
play now pushes simple security policies
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C83C4A-45C4-4285-B791-433FF075165D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A954E4-F638-4D0A-8299-FA034A1EB2B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="FirewallPolicies" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -241,12 +241,6 @@
     <t>Protocol</t>
   </si>
   <si>
-    <t>Portnumbers</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>with Ansible</t>
   </si>
   <si>
@@ -256,9 +250,6 @@
     <t>Untrust</t>
   </si>
   <si>
-    <t>TCP</t>
-  </si>
-  <si>
     <t>DestinationZone</t>
   </si>
   <si>
@@ -305,6 +296,12 @@
   </si>
   <si>
     <t>1000-2000</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>test with ansible</t>
   </si>
 </sst>
 </file>
@@ -674,15 +671,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDA6E7A-D4F7-481D-82C4-1C41B345EEED}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -696,42 +693,36 @@
         <v>63</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>73</v>
-      </c>
-      <c r="H2">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -986,18 +977,18 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1052,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F0D103-70F1-467C-A4A0-6C4FAD2E3DAB}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1071,15 +1062,15 @@
         <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2">
         <v>1234</v>
@@ -1087,10 +1078,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>1234</v>
@@ -1098,10 +1089,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>1456</v>
@@ -1109,13 +1100,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1142,15 +1133,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added application field to the security policy and support for multiple in source/dest and services
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A954E4-F638-4D0A-8299-FA034A1EB2B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A8F172-9E58-40EF-9BD2-5DB708E41CC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -302,6 +302,18 @@
   </si>
   <si>
     <t>test with ansible</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>test1, test3</t>
+  </si>
+  <si>
+    <t>test2, test4</t>
   </si>
 </sst>
 </file>
@@ -671,15 +683,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDA6E7A-D4F7-481D-82C4-1C41B345EEED}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="16.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -699,10 +714,13 @@
         <v>66</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -713,16 +731,19 @@
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
         <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>90</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1065,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1119,7 +1140,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
source and destination zone are now lists
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\pano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B638D0C9-0A48-4A30-992B-F98FFEC2AE2A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B7BCBD-1B74-435C-9AB8-8398C0A4BBC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
@@ -109,12 +109,6 @@
     <t>ifw_coles_1</t>
   </si>
   <si>
-    <t>ifw_internal_1</t>
-  </si>
-  <si>
-    <t>ifw_interbrand_1</t>
-  </si>
-  <si>
     <t>test_source</t>
   </si>
   <si>
@@ -173,6 +167,12 @@
   </si>
   <si>
     <t>tag_name</t>
+  </si>
+  <si>
+    <t>ifw_interbrand_1, ifw_sslvpn_1</t>
+  </si>
+  <si>
+    <t>ifw_internal_1, ifw_sslvpn_1</t>
   </si>
 </sst>
 </file>
@@ -558,18 +558,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDA6E7A-D4F7-481D-82C4-1C41B345EEED}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" customWidth="1"/>
     <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
@@ -583,7 +583,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
@@ -615,22 +615,22 @@
         <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" t="s">
         <v>41</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +662,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -737,34 +737,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -852,10 +852,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Seperated Post and Pre rules, uses role version 2.2.2, all details moved to excel, Pending: Pre-rules
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\pano\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FD304A-FB5E-4A7C-A710-E2FBC5E63C4B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40610C64-C860-4B79-8DAC-1B16EB1A4C4A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="5" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="FirewallPolicies" sheetId="2" r:id="rId1"/>
-    <sheet name="NetworkAddresses" sheetId="1" r:id="rId2"/>
-    <sheet name="NetworkObjects" sheetId="4" r:id="rId3"/>
-    <sheet name="Services" sheetId="5" r:id="rId4"/>
-    <sheet name="ServiceGroups" sheetId="6" r:id="rId5"/>
+    <sheet name="FirewallPolicies_postrule" sheetId="2" r:id="rId1"/>
+    <sheet name="FirewallPolicies_prerule" sheetId="7" r:id="rId2"/>
+    <sheet name="NetworkAddresses" sheetId="1" r:id="rId3"/>
+    <sheet name="NetworkObjects" sheetId="4" r:id="rId4"/>
+    <sheet name="Services" sheetId="5" r:id="rId5"/>
+    <sheet name="ServiceGroups" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -88,9 +89,6 @@
     <t>192.168.96.52</t>
   </si>
   <si>
-    <t>172.22.150.128</t>
-  </si>
-  <si>
     <t>172.22.150.129</t>
   </si>
   <si>
@@ -115,12 +113,6 @@
     <t>test_source</t>
   </si>
   <si>
-    <t>Test_source_1</t>
-  </si>
-  <si>
-    <t>Test_source_2</t>
-  </si>
-  <si>
     <t>test_dest_1</t>
   </si>
   <si>
@@ -151,16 +143,106 @@
     <t>tcp_444, udp_555</t>
   </si>
   <si>
-    <t>tag_name</t>
-  </si>
-  <si>
-    <t>'test_source','Test_source_1'</t>
-  </si>
-  <si>
     <t>'test_source_2'</t>
   </si>
   <si>
-    <t>'test_dest_2','test-dest_3'</t>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>interzone</t>
+  </si>
+  <si>
+    <t>allow</t>
+  </si>
+  <si>
+    <t>spg_au_dc_strict</t>
+  </si>
+  <si>
+    <t>SourceUser</t>
+  </si>
+  <si>
+    <t>HIPProfile</t>
+  </si>
+  <si>
+    <t>URLCategory</t>
+  </si>
+  <si>
+    <t>SecurityProfile</t>
+  </si>
+  <si>
+    <t>PostRule</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>LogStart</t>
+  </si>
+  <si>
+    <t>LogEnd</t>
+  </si>
+  <si>
+    <t>LogSettings</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>test, test2</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>Devicegroup</t>
+  </si>
+  <si>
+    <t>Existing_rule</t>
+  </si>
+  <si>
+    <t>172.22.150.128-172.22.150.192</t>
+  </si>
+  <si>
+    <t>test_source_1</t>
+  </si>
+  <si>
+    <t>test_source_2</t>
+  </si>
+  <si>
+    <t>'test_source','test_source_1'</t>
+  </si>
+  <si>
+    <t>'test_dest_2','test_dest_3'</t>
+  </si>
+  <si>
+    <t>tcp_9999</t>
+  </si>
+  <si>
+    <t>service_group2</t>
   </si>
 </sst>
 </file>
@@ -216,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -230,6 +312,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,143 +629,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDA6E7A-D4F7-481D-82C4-1C41B345EEED}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" customWidth="1"/>
-    <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="30.88671875" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2"/>
+      <c r="L2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2D0E66-9821-4420-9073-ECB8C986F385}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E16442-E7CB-4AA7-B35A-4998D89832EC}">
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" customWidth="1"/>
+    <col min="12" max="12" width="21.21875" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" customWidth="1"/>
+    <col min="17" max="17" width="20.109375" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" customWidth="1"/>
+    <col min="20" max="20" width="16.109375" customWidth="1"/>
+    <col min="21" max="21" width="15.44140625" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
+    <col min="23" max="23" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -689,60 +906,245 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2D0E66-9821-4420-9073-ECB8C986F385}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E769B2-D3A4-44F7-90E9-E6DD516C6612}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
     </row>
   </sheetData>
@@ -751,12 +1153,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F0D103-70F1-467C-A4A0-6C4FAD2E3DAB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,9 +1166,12 @@
     <col min="1" max="1" width="18.88671875" customWidth="1"/>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -776,8 +1181,17 @@
       <c r="C1" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A3" si="0">_xlfn.CONCAT(LOWER(B2),"_",C2)</f>
         <v>tcp_444</v>
@@ -788,8 +1202,17 @@
       <c r="C2">
         <v>444</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>udp_555</v>
@@ -799,6 +1222,35 @@
       </c>
       <c r="C3">
         <v>555</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>9999</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -806,34 +1258,71 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6472A306-4237-4364-B563-EDDE513583A6}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted post rule check from Excel,Template and variables, Set to true in the task
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40610C64-C860-4B79-8DAC-1B16EB1A4C4A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A135081-7568-4FD9-86BC-D5D186363795}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="5" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="FirewallPolicies_postrule" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -188,9 +188,6 @@
     <t>SecurityProfile</t>
   </si>
   <si>
-    <t>PostRule</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>service_group2</t>
+  </si>
+  <si>
+    <t>delete</t>
   </si>
 </sst>
 </file>
@@ -629,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDA6E7A-D4F7-481D-82C4-1C41B345EEED}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,9 +653,9 @@
     <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -664,7 +664,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>38</v>
@@ -709,24 +709,21 @@
         <v>41</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>42</v>
@@ -741,28 +738,28 @@
         <v>22</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>44</v>
@@ -777,9 +774,6 @@
         <v>1</v>
       </c>
       <c r="T2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -793,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E16442-E7CB-4AA7-B35A-4998D89832EC}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +820,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -835,7 +829,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>38</v>
@@ -883,21 +877,21 @@
         <v>36</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -910,132 +904,133 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1048,104 +1043,104 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
       <c r="D5" t="s">
         <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1157,100 +1152,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F0D103-70F1-467C-A4A0-6C4FAD2E3DAB}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="E1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f t="shared" ref="A2:A3" si="0">_xlfn.CONCAT(LOWER(B2),"_",C2)</f>
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B3" si="0">_xlfn.CONCAT(LOWER(C2),"_",D2)</f>
         <v>tcp_444</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>444</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
       <c r="E2" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="str">
         <f t="shared" si="0"/>
         <v>udp_555</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>555</v>
       </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
       <c r="E3" t="s">
         <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>9999</v>
       </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
       <c r="E4" t="s">
         <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1262,50 +1257,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6472A306-4237-4364-B563-EDDE513583A6}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1316,13 +1311,13 @@
         <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added support for pre-rules
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A135081-7568-4FD9-86BC-D5D186363795}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22B915D-BCC2-43CA-A978-B0AA136C9863}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="FirewallPolicies_postrule" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -200,9 +200,6 @@
     <t>LogEnd</t>
   </si>
   <si>
-    <t>LogSettings</t>
-  </si>
-  <si>
     <t>Operation</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>Devicegroup</t>
   </si>
   <si>
-    <t>Existing_rule</t>
-  </si>
-  <si>
     <t>172.22.150.128-172.22.150.192</t>
   </si>
   <si>
@@ -242,7 +236,25 @@
     <t>service_group2</t>
   </si>
   <si>
-    <t>delete</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>ExistingRule</t>
+  </si>
+  <si>
+    <t>LogSetting</t>
+  </si>
+  <si>
+    <t>lf_au_dc_panorama</t>
+  </si>
+  <si>
+    <t>Deny</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>update</t>
   </si>
 </sst>
 </file>
@@ -631,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDA6E7A-D4F7-481D-82C4-1C41B345EEED}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="J1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,7 +667,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -664,7 +676,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>38</v>
@@ -717,7 +729,7 @@
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
@@ -741,10 +753,10 @@
         <v>51</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
@@ -787,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E16442-E7CB-4AA7-B35A-4998D89832EC}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,12 +827,12 @@
     <col min="20" max="20" width="16.109375" customWidth="1"/>
     <col min="21" max="21" width="15.44140625" customWidth="1"/>
     <col min="22" max="22" width="11.6640625" customWidth="1"/>
-    <col min="23" max="23" width="12.88671875" customWidth="1"/>
+    <col min="23" max="23" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -829,7 +841,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>38</v>
@@ -877,7 +889,7 @@
         <v>36</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>52</v>
@@ -886,12 +898,78 @@
         <v>53</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>56</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -904,7 +982,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,7 +994,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -925,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -933,7 +1011,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -950,10 +1028,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -967,13 +1045,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -984,7 +1062,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1001,7 +1079,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -1018,7 +1096,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -1043,7 +1121,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,7 +1134,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1065,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -1073,13 +1151,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>42</v>
@@ -1090,7 +1168,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>29</v>
@@ -1107,7 +1185,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
@@ -1124,13 +1202,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -1153,7 +1231,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,7 +1246,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1180,7 +1258,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -1188,7 +1266,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B3" si="0">_xlfn.CONCAT(LOWER(C2),"_",D2)</f>
@@ -1209,7 +1287,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
@@ -1230,10 +1308,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -1258,7 +1336,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1271,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1280,7 +1358,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
@@ -1288,7 +1366,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -1305,13 +1383,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
fixed URL catefory for post rule, and tested pre-rule
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22B915D-BCC2-43CA-A978-B0AA136C9863}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03526DAD-62F1-4B77-93F8-9E7A4321FCCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="FirewallPolicies_postrule" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -245,16 +245,13 @@
     <t>LogSetting</t>
   </si>
   <si>
+    <t>top</t>
+  </si>
+  <si>
     <t>lf_au_dc_panorama</t>
   </si>
   <si>
-    <t>Deny</t>
-  </si>
-  <si>
-    <t>before</t>
-  </si>
-  <si>
-    <t>update</t>
+    <t>adult</t>
   </si>
 </sst>
 </file>
@@ -643,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDA6E7A-D4F7-481D-82C4-1C41B345EEED}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -765,7 +762,7 @@
         <v>51</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>51</v>
@@ -799,14 +796,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E16442-E7CB-4AA7-B35A-4998D89832EC}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
@@ -902,9 +899,6 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
@@ -957,11 +951,9 @@
         <v>66</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="T2" s="1"/>
       <c r="U2" s="1" t="b">
         <v>1</v>
       </c>
@@ -969,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="W2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
log messages are now written to a csv with clear indication if it was successful or failure
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F98D8A9-1CCA-4F2C-97F7-83A578EEAAD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E785379-1891-47B2-BA71-48AA6D2B484D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="753" activeTab="2" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="753" activeTab="3" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="FirewallPolicies_postrule" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="205">
   <si>
     <t>Name</t>
   </si>
@@ -278,21 +278,12 @@
     <t>ifw-coles_1</t>
   </si>
   <si>
-    <t>grp_intranet_portal</t>
-  </si>
-  <si>
     <t>hoc_172.25.151.51_utnnm, hoc_172.25.151.52_utnnm</t>
   </si>
   <si>
     <t>hoc_172.27.255.84_idmutils</t>
   </si>
   <si>
-    <t>grp_coles_intsmtp</t>
-  </si>
-  <si>
-    <t>grp_coles_serverfarm</t>
-  </si>
-  <si>
     <t>noc_172.28.0.0_coles_dev</t>
   </si>
   <si>
@@ -300,9 +291,6 @@
   </si>
   <si>
     <t>hoc_172.25.184.159_coleswebmail, hoc_172.27.0.135_webmail.cmltd.net.au, hoc_172.27.0.136_as3g.coles.com.au</t>
-  </si>
-  <si>
-    <t>grp_proxy-int_intfc</t>
   </si>
   <si>
     <t>tcp_464, udp_123, udp_389, udp_464, udp_636, udp_88, udp_138, tcp_135, tcp_139, tcp_3268, tcp_445, tcp_88</t>
@@ -393,37 +381,13 @@
     <t>nok_172.31.0.0-16_KmartHO</t>
   </si>
   <si>
-    <t>Colesall</t>
-  </si>
-  <si>
-    <t>del_172.22.61.243_utsap1</t>
-  </si>
-  <si>
-    <t>del_172.22.61.30_sh0301ec</t>
-  </si>
-  <si>
     <t>gpc_qet_servers</t>
   </si>
   <si>
-    <t>gpc_wins</t>
-  </si>
-  <si>
     <t>grp_coles_prod_mq</t>
   </si>
   <si>
-    <t>grp_Coles_Tivoli_Servers</t>
-  </si>
-  <si>
-    <t>grp_internal_dns</t>
-  </si>
-  <si>
-    <t>grp_SAP_new</t>
-  </si>
-  <si>
     <t>grp_sysmanage_servers</t>
-  </si>
-  <si>
-    <t>grp_TRM_servers</t>
   </si>
   <si>
     <t>grp_Windows_Filesystems</t>
@@ -646,30 +610,6 @@
     <t>hoc_172.22.161.23_lx-papcops, hoc_172.22.161.72, hoc_172.22.162.61_APCDCO</t>
   </si>
   <si>
-    <t>same</t>
-  </si>
-  <si>
-    <t>goc_qet_servers</t>
-  </si>
-  <si>
-    <t>goc_wins</t>
-  </si>
-  <si>
-    <t>object not present</t>
-  </si>
-  <si>
-    <t>goc_coles_tivoli_servers</t>
-  </si>
-  <si>
-    <t>goc_internal_dns</t>
-  </si>
-  <si>
-    <t>goc_trm_servers</t>
-  </si>
-  <si>
-    <t>goc_windows_filesystems</t>
-  </si>
-  <si>
     <t>tcp_3333</t>
   </si>
   <si>
@@ -695,6 +635,24 @@
   </si>
   <si>
     <t>172.22.150.128/25</t>
+  </si>
+  <si>
+    <t>goc_test</t>
+  </si>
+  <si>
+    <t>'hoc_test', 'hoc_test2'</t>
+  </si>
+  <si>
+    <t>'hoc_test', 'hoc_test2', 'hoc_test3'</t>
+  </si>
+  <si>
+    <t>goc_fail</t>
+  </si>
+  <si>
+    <t>'hoc_test', 'hoc_test2', 'hoc_test5'</t>
+  </si>
+  <si>
+    <t>goc_test1</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1152,7 @@
         <v>63</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>18</v>
@@ -1206,7 +1164,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>36</v>
@@ -1218,7 +1176,7 @@
         <v>79</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>36</v>
@@ -1227,7 +1185,7 @@
         <v>36</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>29</v>
@@ -1256,7 +1214,7 @@
         <v>64</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>18</v>
@@ -1268,7 +1226,7 @@
         <v>77</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>36</v>
@@ -1280,7 +1238,7 @@
         <v>79</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>36</v>
@@ -1289,7 +1247,7 @@
         <v>36</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>29</v>
@@ -1318,7 +1276,7 @@
         <v>65</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>18</v>
@@ -1330,7 +1288,7 @@
         <v>77</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>36</v>
@@ -1342,7 +1300,7 @@
         <v>79</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>36</v>
@@ -1351,7 +1309,7 @@
         <v>36</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>29</v>
@@ -1380,7 +1338,7 @@
         <v>66</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>18</v>
@@ -1392,7 +1350,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>36</v>
@@ -1404,7 +1362,7 @@
         <v>79</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>36</v>
@@ -1413,7 +1371,7 @@
         <v>36</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>29</v>
@@ -1442,7 +1400,7 @@
         <v>67</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>18</v>
@@ -1454,7 +1412,7 @@
         <v>77</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>36</v>
@@ -1466,7 +1424,7 @@
         <v>79</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>36</v>
@@ -1475,7 +1433,7 @@
         <v>36</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>29</v>
@@ -1504,7 +1462,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>18</v>
@@ -1516,7 +1474,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>36</v>
@@ -1528,7 +1486,7 @@
         <v>79</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>36</v>
@@ -1537,7 +1495,7 @@
         <v>36</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>29</v>
@@ -1566,7 +1524,7 @@
         <v>69</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>18</v>
@@ -1578,7 +1536,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>36</v>
@@ -1590,7 +1548,7 @@
         <v>79</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M8" s="8" t="s">
         <v>36</v>
@@ -1599,7 +1557,7 @@
         <v>36</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>29</v>
@@ -1628,7 +1586,7 @@
         <v>70</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>18</v>
@@ -1640,7 +1598,7 @@
         <v>19</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>36</v>
@@ -1652,7 +1610,7 @@
         <v>79</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>36</v>
@@ -1661,7 +1619,7 @@
         <v>36</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>29</v>
@@ -1690,7 +1648,7 @@
         <v>71</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>18</v>
@@ -1702,7 +1660,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>36</v>
@@ -1714,7 +1672,7 @@
         <v>79</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>36</v>
@@ -1723,7 +1681,7 @@
         <v>36</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>29</v>
@@ -1752,7 +1710,7 @@
         <v>72</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>18</v>
@@ -1764,7 +1722,7 @@
         <v>77</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>36</v>
@@ -1776,7 +1734,7 @@
         <v>79</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>36</v>
@@ -1785,7 +1743,7 @@
         <v>36</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>29</v>
@@ -1814,7 +1772,7 @@
         <v>73</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>18</v>
@@ -1838,7 +1796,7 @@
         <v>79</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M12" s="8" t="s">
         <v>36</v>
@@ -1876,7 +1834,7 @@
         <v>74</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>18</v>
@@ -1888,7 +1846,7 @@
         <v>19</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>36</v>
@@ -1900,7 +1858,7 @@
         <v>79</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M13" s="8" t="s">
         <v>36</v>
@@ -1909,7 +1867,7 @@
         <v>36</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="P13" s="8" t="s">
         <v>29</v>
@@ -1938,7 +1896,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>18</v>
@@ -1950,7 +1908,7 @@
         <v>19</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>36</v>
@@ -1962,7 +1920,7 @@
         <v>79</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M14" s="8" t="s">
         <v>36</v>
@@ -1971,7 +1929,7 @@
         <v>36</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P14" s="8" t="s">
         <v>29</v>
@@ -2000,7 +1958,7 @@
         <v>76</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>18</v>
@@ -2012,7 +1970,7 @@
         <v>19</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>36</v>
@@ -2024,7 +1982,7 @@
         <v>79</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>36</v>
@@ -2033,7 +1991,7 @@
         <v>36</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="P15" s="8" t="s">
         <v>29</v>
@@ -2053,13 +2011,13 @@
     </row>
     <row r="16" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>18</v>
@@ -2068,7 +2026,7 @@
         <v>77</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>36</v>
@@ -2080,7 +2038,7 @@
         <v>79</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>36</v>
@@ -2089,7 +2047,7 @@
         <v>36</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P16" s="8" t="s">
         <v>29</v>
@@ -2109,13 +2067,13 @@
     </row>
     <row r="17" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>18</v>
@@ -2124,7 +2082,7 @@
         <v>19</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>36</v>
@@ -2136,7 +2094,7 @@
         <v>79</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="M17" s="8" t="s">
         <v>36</v>
@@ -2145,7 +2103,7 @@
         <v>36</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>29</v>
@@ -2165,13 +2123,13 @@
     </row>
     <row r="18" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>18</v>
@@ -2180,7 +2138,7 @@
         <v>19</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>36</v>
@@ -2192,7 +2150,7 @@
         <v>79</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>36</v>
@@ -2201,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="P18" s="8" t="s">
         <v>29</v>
@@ -2221,13 +2179,13 @@
     </row>
     <row r="19" spans="2:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>18</v>
@@ -2236,7 +2194,7 @@
         <v>19</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>36</v>
@@ -2248,7 +2206,7 @@
         <v>79</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="M19" s="8" t="s">
         <v>36</v>
@@ -2257,7 +2215,7 @@
         <v>36</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>29</v>
@@ -2277,13 +2235,13 @@
     </row>
     <row r="20" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>18</v>
@@ -2292,7 +2250,7 @@
         <v>19</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>36</v>
@@ -2304,16 +2262,16 @@
         <v>79</v>
       </c>
       <c r="L20" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O20" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O20" s="8" t="s">
-        <v>184</v>
       </c>
       <c r="P20" s="8" t="s">
         <v>29</v>
@@ -2333,13 +2291,13 @@
     </row>
     <row r="21" spans="2:20" ht="144" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>18</v>
@@ -2348,7 +2306,7 @@
         <v>77</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>36</v>
@@ -2360,16 +2318,16 @@
         <v>79</v>
       </c>
       <c r="L21" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O21" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="P21" s="8" t="s">
         <v>29</v>
@@ -2389,13 +2347,13 @@
     </row>
     <row r="22" spans="2:20" ht="144" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>18</v>
@@ -2404,7 +2362,7 @@
         <v>19</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>36</v>
@@ -2416,16 +2374,16 @@
         <v>79</v>
       </c>
       <c r="L22" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O22" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O22" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="P22" s="8" t="s">
         <v>29</v>
@@ -2445,13 +2403,13 @@
     </row>
     <row r="23" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>18</v>
@@ -2460,7 +2418,7 @@
         <v>19</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>36</v>
@@ -2472,16 +2430,16 @@
         <v>79</v>
       </c>
       <c r="L23" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O23" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O23" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="P23" s="8" t="s">
         <v>29</v>
@@ -2501,13 +2459,13 @@
     </row>
     <row r="24" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>18</v>
@@ -2516,7 +2474,7 @@
         <v>77</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>36</v>
@@ -2528,16 +2486,16 @@
         <v>79</v>
       </c>
       <c r="L24" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O24" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N24" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O24" s="8" t="s">
-        <v>188</v>
       </c>
       <c r="P24" s="8" t="s">
         <v>29</v>
@@ -2557,13 +2515,13 @@
     </row>
     <row r="25" spans="2:20" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>18</v>
@@ -2572,7 +2530,7 @@
         <v>77</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>36</v>
@@ -2584,16 +2542,16 @@
         <v>79</v>
       </c>
       <c r="L25" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O25" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O25" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="P25" s="8" t="s">
         <v>29</v>
@@ -2613,13 +2571,13 @@
     </row>
     <row r="26" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>18</v>
@@ -2628,7 +2586,7 @@
         <v>19</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>36</v>
@@ -2640,7 +2598,7 @@
         <v>79</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>36</v>
@@ -2649,7 +2607,7 @@
         <v>36</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="P26" s="8" t="s">
         <v>29</v>
@@ -2669,13 +2627,13 @@
     </row>
     <row r="27" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>18</v>
@@ -2684,7 +2642,7 @@
         <v>77</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>36</v>
@@ -2696,7 +2654,7 @@
         <v>79</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="M27" s="8" t="s">
         <v>36</v>
@@ -2705,7 +2663,7 @@
         <v>36</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="P27" s="8" t="s">
         <v>29</v>
@@ -2725,13 +2683,13 @@
     </row>
     <row r="28" spans="2:20" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>18</v>
@@ -2740,7 +2698,7 @@
         <v>77</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>36</v>
@@ -2752,7 +2710,7 @@
         <v>79</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="M28" s="8" t="s">
         <v>36</v>
@@ -2761,7 +2719,7 @@
         <v>36</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="P28" s="8" t="s">
         <v>29</v>
@@ -2781,13 +2739,13 @@
     </row>
     <row r="29" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>18</v>
@@ -2796,7 +2754,7 @@
         <v>77</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>36</v>
@@ -2808,7 +2766,7 @@
         <v>79</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="M29" s="8" t="s">
         <v>36</v>
@@ -2817,7 +2775,7 @@
         <v>36</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="P29" s="8" t="s">
         <v>29</v>
@@ -2837,13 +2795,13 @@
     </row>
     <row r="30" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>18</v>
@@ -2852,7 +2810,7 @@
         <v>19</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>36</v>
@@ -2864,7 +2822,7 @@
         <v>79</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="M30" s="8" t="s">
         <v>36</v>
@@ -2873,7 +2831,7 @@
         <v>36</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="P30" s="8" t="s">
         <v>29</v>
@@ -2893,13 +2851,13 @@
     </row>
     <row r="31" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>18</v>
@@ -2908,7 +2866,7 @@
         <v>19</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>36</v>
@@ -2920,7 +2878,7 @@
         <v>79</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="M31" s="8" t="s">
         <v>36</v>
@@ -2929,7 +2887,7 @@
         <v>36</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P31" s="8" t="s">
         <v>29</v>
@@ -2949,13 +2907,13 @@
     </row>
     <row r="32" spans="2:20" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>18</v>
@@ -2964,7 +2922,7 @@
         <v>19</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>36</v>
@@ -2976,7 +2934,7 @@
         <v>79</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="M32" s="8" t="s">
         <v>36</v>
@@ -2985,7 +2943,7 @@
         <v>36</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="P32" s="8" t="s">
         <v>29</v>
@@ -3005,13 +2963,13 @@
     </row>
     <row r="33" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>18</v>
@@ -3020,7 +2978,7 @@
         <v>77</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>36</v>
@@ -3032,7 +2990,7 @@
         <v>79</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="M33" s="8" t="s">
         <v>36</v>
@@ -3041,7 +2999,7 @@
         <v>36</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="P33" s="8" t="s">
         <v>29</v>
@@ -3061,13 +3019,13 @@
     </row>
     <row r="34" spans="2:20" ht="72" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>18</v>
@@ -3076,7 +3034,7 @@
         <v>19</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>36</v>
@@ -3088,7 +3046,7 @@
         <v>79</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>36</v>
@@ -3097,7 +3055,7 @@
         <v>36</v>
       </c>
       <c r="O34" s="8" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="P34" s="8" t="s">
         <v>29</v>
@@ -3302,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2D0E66-9821-4420-9073-ECB8C986F385}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3336,13 +3294,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -3350,13 +3308,13 @@
         <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3364,13 +3322,13 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3378,13 +3336,13 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3394,17 +3352,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E769B2-D3A4-44F7-90E9-E6DD516C6612}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="35.109375" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3426,139 +3384,45 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
       <c r="B2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="7"/>
+        <v>199</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
       <c r="B3" s="8" t="s">
-        <v>119</v>
+        <v>204</v>
+      </c>
+      <c r="C3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
       <c r="B4" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" t="s">
-        <v>209</v>
+      <c r="D4" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3620,7 +3484,7 @@
         <v>464</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -3638,7 +3502,7 @@
         <v>123</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3646,7 +3510,7 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -3655,15 +3519,15 @@
         <v>3333</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -3672,7 +3536,7 @@
         <v>4444</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pre and post rules are now handled in the same function, add and update are split out
</commit_message>
<xml_diff>
--- a/variables/configuration.xlsx
+++ b/variables/configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudarshanVijayaKumar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudarshanv/Documents/Projects/panorama/variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E785379-1891-47B2-BA71-48AA6D2B484D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15E5EFA-50A5-7C47-9D03-6FFD3246701E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="753" activeTab="3" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" tabRatio="753" activeTab="1" xr2:uid="{14BF9E76-722D-4A72-8D6C-E94CE9EBBE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="FirewallPolicies_postrule" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="205">
   <si>
     <t>Name</t>
   </si>
@@ -1058,28 +1058,28 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="8"/>
-    <col min="2" max="2" width="27.44140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="8"/>
+    <col min="2" max="2" width="27.5" style="8" customWidth="1"/>
     <col min="3" max="3" width="19" style="8" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" style="8" customWidth="1"/>
     <col min="9" max="10" width="26" style="8" customWidth="1"/>
-    <col min="11" max="11" width="30.88671875" style="8" customWidth="1"/>
-    <col min="12" max="12" width="47.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" style="8" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" style="8"/>
+    <col min="11" max="11" width="30.83203125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="47.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.1640625" style="8" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5" style="8"/>
     <col min="17" max="17" width="19" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="14.44140625" style="8"/>
+    <col min="18" max="16384" width="14.5" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>39</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>40</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="224" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>40</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>40</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>40</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>40</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>40</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>40</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>40</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>40</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>40</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>40</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>118</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" ht="80" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>119</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
         <v>120</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" ht="144" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>121</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>122</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="144" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" ht="160" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>123</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="144" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" ht="160" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
         <v>124</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" ht="80" x14ac:dyDescent="0.2">
       <c r="B23" s="8" t="s">
         <v>125</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>126</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>127</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>128</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
         <v>129</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" ht="176" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
         <v>130</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B29" s="8" t="s">
         <v>131</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B30" s="8" t="s">
         <v>132</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B31" s="8" t="s">
         <v>133</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" ht="80" x14ac:dyDescent="0.2">
       <c r="B32" s="8" t="s">
         <v>134</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B33" s="8" t="s">
         <v>135</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:20" ht="64" x14ac:dyDescent="0.2">
       <c r="B34" s="8" t="s">
         <v>136</v>
       </c>
@@ -3083,38 +3083,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E16442-E7CB-4AA7-B35A-4998D89832EC}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" customWidth="1"/>
-    <col min="12" max="12" width="21.21875" customWidth="1"/>
-    <col min="13" max="13" width="21.109375" customWidth="1"/>
-    <col min="14" max="14" width="19.109375" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" customWidth="1"/>
-    <col min="17" max="17" width="20.109375" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" customWidth="1"/>
+    <col min="12" max="13" width="21.1640625" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" customWidth="1"/>
+    <col min="16" max="16" width="19.1640625" customWidth="1"/>
+    <col min="17" max="17" width="20.1640625" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
-    <col min="20" max="20" width="16.109375" customWidth="1"/>
-    <col min="21" max="21" width="15.44140625" customWidth="1"/>
+    <col min="19" max="19" width="13.5" customWidth="1"/>
+    <col min="20" max="20" width="16.1640625" customWidth="1"/>
+    <col min="21" max="21" width="15.5" customWidth="1"/>
     <col min="22" max="22" width="11.6640625" customWidth="1"/>
-    <col min="23" max="23" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -3185,7 +3184,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3264,15 +3266,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -3289,7 +3291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3303,7 +3305,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3317,7 +3319,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3331,7 +3333,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -3354,19 +3356,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E769B2-D3A4-44F7-90E9-E6DD516C6612}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -3383,7 +3385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3397,7 +3399,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3411,7 +3413,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3439,17 +3441,17 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>39</v>
       </c>
@@ -3469,7 +3471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3487,7 +3489,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3505,7 +3507,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3522,7 +3524,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>191</v>
       </c>
@@ -3552,15 +3554,15 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>39</v>
       </c>
@@ -3577,7 +3579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" s="3"/>
     </row>
   </sheetData>

</xml_diff>